<commit_message>
More PreSuperFrom experimenting and updated research hours
</commit_message>
<xml_diff>
--- a/AT/Research Hours.xlsx
+++ b/AT/Research Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailtouma/Desktop/SSS-Experiments/AT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19CA6351-3C20-1247-8AEF-180DF9F811CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8361B584-A22A-274A-8060-E80D0A82F6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="740" windowWidth="27640" windowHeight="16940" xr2:uid="{9D7B63EE-5957-9947-A3B5-024424A2FDD1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>meeting - worked on PreSuperForm</t>
+  </si>
+  <si>
+    <t>continued experimenting with PreSuperForm</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7542DF9F-5D83-964C-81A0-40C880F500E5}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -469,7 +472,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -498,8 +501,8 @@
         <v>1.25</v>
       </c>
       <c r="E2" s="3">
-        <f>SUM(C2:C12)</f>
-        <v>10.33</v>
+        <f>SUM(C2:C13)</f>
+        <v>11.08</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -610,6 +613,17 @@
       </c>
       <c r="C12">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>46055</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated research hours and PreSuperForm doc
</commit_message>
<xml_diff>
--- a/AT/Research Hours.xlsx
+++ b/AT/Research Hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailtouma/Desktop/SSS-Experiments/AT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C98F1D1E-3BDF-F54A-9C3A-627460C2BC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C7C2984-1D79-BC4B-A28C-3342C502E9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="740" windowWidth="27640" windowHeight="16940" xr2:uid="{9D7B63EE-5957-9947-A3B5-024424A2FDD1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>meeting - continued looking for patterns</t>
+  </si>
+  <si>
+    <t>created more examples to recognize patterns</t>
   </si>
 </sst>
 </file>
@@ -88,7 +91,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -131,7 +134,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -147,10 +150,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,19 +469,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7542DF9F-5D83-964C-81A0-40C880F500E5}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,8 +495,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45996</v>
       </c>
@@ -507,11 +508,11 @@
         <v>1.25</v>
       </c>
       <c r="E2" s="3">
-        <f>SUM(C2:C16)</f>
-        <v>13.08</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <f>SUM(C2:C17)</f>
+        <v>13.83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45996</v>
       </c>
@@ -522,7 +523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>46034</v>
       </c>
@@ -533,7 +534,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>46036</v>
       </c>
@@ -544,7 +545,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>46038</v>
       </c>
@@ -555,7 +556,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>46041</v>
       </c>
@@ -566,7 +567,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>46041</v>
       </c>
@@ -577,7 +578,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>46048</v>
       </c>
@@ -588,7 +589,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>46050</v>
       </c>
@@ -599,7 +600,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>46051</v>
       </c>
@@ -610,7 +611,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>46055</v>
       </c>
@@ -621,7 +622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>46055</v>
       </c>
@@ -632,7 +633,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>46059</v>
       </c>
@@ -643,7 +644,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>46060</v>
       </c>
@@ -654,7 +655,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>46062</v>
       </c>
@@ -663,6 +664,17 @@
       </c>
       <c r="C16">
         <v>1.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>46071</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more examples, a potential rule for odd I-Cats, and updated research hours
</commit_message>
<xml_diff>
--- a/AT/Research Hours.xlsx
+++ b/AT/Research Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailtouma/Desktop/SSS-Experiments/AT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D88AEB5-D8AC-AC43-B3E0-347BC76654C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A727296-7C0D-CF4F-A791-9BB39104402D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="740" windowWidth="27640" windowHeight="16940" xr2:uid="{9D7B63EE-5957-9947-A3B5-024424A2FDD1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>meeting -  formed some hypotheses</t>
+  </si>
+  <si>
+    <t>worked on the hypothesis - U=M/C</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7542DF9F-5D83-964C-81A0-40C880F500E5}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,6 +708,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>46079</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated research hours and continued working on examples
</commit_message>
<xml_diff>
--- a/AT/Research Hours.xlsx
+++ b/AT/Research Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailtouma/Desktop/SSS-Experiments/AT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A727296-7C0D-CF4F-A791-9BB39104402D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4FFC30A-3053-8644-816F-2F7660A7065F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="740" windowWidth="27640" windowHeight="16940" xr2:uid="{9D7B63EE-5957-9947-A3B5-024424A2FDD1}"/>
   </bookViews>
@@ -481,7 +481,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,8 +517,8 @@
         <v>1.25</v>
       </c>
       <c r="E2" s="3">
-        <f>SUM(C2:C19)</f>
-        <v>15.16</v>
+        <f>SUM(C2:C20)</f>
+        <v>16.66</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -716,7 +716,7 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>